<commit_message>
remains the group private
</commit_message>
<xml_diff>
--- a/src/assets/birthdays.xlsx
+++ b/src/assets/birthdays.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\New folder\pibbox_birthdays\src\pibox_birthdays\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\New folder\pibbox_birthdays\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC31D3A-C1A0-4FBF-93EA-70FD4FC659F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916CFEA8-4621-4CD8-973E-8ED5BCCF2A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>08.02</t>
-  </si>
-  <si>
     <t>פלוני אלמוני</t>
   </si>
   <si>
@@ -32,6 +29,9 @@
   </si>
   <si>
     <t>ישראל ישראלי</t>
+  </si>
+  <si>
+    <t>09.02</t>
   </si>
 </sst>
 </file>
@@ -377,7 +377,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -388,18 +388,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>